<commit_message>
test reference constants file added
</commit_message>
<xml_diff>
--- a/test/test_reference_values.xlsx
+++ b/test/test_reference_values.xlsx
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,6 +571,7 @@
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -600,7 +601,7 @@
       <c r="B3" s="2">
         <v>1E+21</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <f>LOG10(B3)-20</f>
         <v>1</v>
       </c>
@@ -612,7 +613,7 @@
       <c r="B4" s="2">
         <v>100000</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <f>LOG10(B4)-3</f>
         <v>2</v>
       </c>
@@ -625,7 +626,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="D6">
+      <c r="D6" s="3">
         <f>14.9-0.5*(D3)+D4</f>
         <v>16.399999999999999</v>
       </c>

</xml_diff>

<commit_message>
new calculations added to the excel file
</commit_message>
<xml_diff>
--- a/test/test_reference_values.xlsx
+++ b/test/test_reference_values.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RUNAFLUID_phys_numbers" sheetId="1" r:id="rId1"/>
+    <sheet name="Aval_thresh_gen_rate" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="95">
   <si>
     <t>14.9 - 0.5 * log(electron_density * 1e-20) + log(electron_temperature * 1e-3);</t>
   </si>
@@ -211,17 +212,111 @@
   </si>
   <si>
     <t>dreicer_growth_rate_67</t>
+  </si>
+  <si>
+    <t>Value:</t>
+  </si>
+  <si>
+    <t>Function name:</t>
+  </si>
+  <si>
+    <t>Electron density</t>
+  </si>
+  <si>
+    <t>Electron's charge</t>
+  </si>
+  <si>
+    <t>π</t>
+  </si>
+  <si>
+    <t>Epsilon_0</t>
+  </si>
+  <si>
+    <t>Electron's mass</t>
+  </si>
+  <si>
+    <t>4*π*Eps0^2</t>
+  </si>
+  <si>
+    <t>Speed of light( c )</t>
+  </si>
+  <si>
+    <t>Columb lambda</t>
+  </si>
+  <si>
+    <t>Ne*e^3*Ln(lambda)</t>
+  </si>
+  <si>
+    <t>Electron temperature in Joule</t>
+  </si>
+  <si>
+    <t>Electron temperature in eV</t>
+  </si>
+  <si>
+    <t>Sqrt(8)</t>
+  </si>
+  <si>
+    <t>Effective charge(Zeff)</t>
+  </si>
+  <si>
+    <t>e^4</t>
+  </si>
+  <si>
+    <t>Ne*Ln(lambda)</t>
+  </si>
+  <si>
+    <t>Runaway electron collision time</t>
+  </si>
+  <si>
+    <t>M0^2*c^3</t>
+  </si>
+  <si>
+    <t>M0*c^2</t>
+  </si>
+  <si>
+    <t>6*π*Eps0*M0*c^3</t>
+  </si>
+  <si>
+    <t>Variable/calculations name:</t>
+  </si>
+  <si>
+    <t>e^4*B^2</t>
+  </si>
+  <si>
+    <t>Magnetic field</t>
+  </si>
+  <si>
+    <t>Synchrotron loss time</t>
+  </si>
+  <si>
+    <t>Normalised synchrotron loss time</t>
+  </si>
+  <si>
+    <t>Avalanche threshold electric field</t>
+  </si>
+  <si>
+    <t>(Zeff+1)/sqrt(Trad)</t>
+  </si>
+  <si>
+    <t>1/8+(Zeff+1)^2/Trad</t>
+  </si>
+  <si>
+    <t>Sixth square(1/8+(Zeff+1)^2/Trad)</t>
+  </si>
+  <si>
+    <t>Lambda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00E+000"/>
     <numFmt numFmtId="165" formatCode="0.0000E+000"/>
+    <numFmt numFmtId="169" formatCode="0.00000E+00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,13 +329,33 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF26E62F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -270,22 +385,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF26E62F"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -559,11 +685,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +702,7 @@
     <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -630,41 +756,41 @@
         <f>14.9-0.5*(D3)+D4</f>
         <v>16.399999999999999</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="9">
         <f>D6</f>
         <v>16.399999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="10">
         <v>1.6021766200000001E-19</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="9">
         <f>B7^3</f>
         <v>4.1127391927503151E-57</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="9">
         <f>PI()</f>
         <v>3.1415926535897931</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="9">
         <f>B11^3</f>
         <v>2.6944002417373989E+25</v>
       </c>
@@ -677,49 +803,52 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="11">
         <v>8.8541878169999989E-12</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="9">
         <f>B14</f>
         <v>6.744892276110516E-35</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="9">
         <f>H6*H7*B3</f>
         <v>6.744892276110516E-35</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="11">
         <v>9.1093835599999998E-31</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="9">
         <f>B10</f>
         <v>9.1093835599999998E-31</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="11">
         <v>299792458</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
+      <c r="B12" s="3">
+        <f>RUNAFLUID_phys_numbers!B1</f>
+        <v>0</v>
+      </c>
       <c r="G12" t="s">
         <v>15</v>
       </c>
@@ -731,10 +860,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
-      <c r="G13" t="s">
+      <c r="G13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="9">
         <f>B15</f>
         <v>9.8516125702040363E-22</v>
       </c>
@@ -747,10 +876,10 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="9">
         <f>B3*B7^3*D6</f>
         <v>6.744892276110516E-35</v>
       </c>
@@ -763,19 +892,19 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="9">
         <f>4*B8*B9*B9</f>
         <v>9.8516125702040363E-22</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="9">
         <f>B10*B11*B11</f>
         <v>8.1871056496500277E-14</v>
       </c>
@@ -1070,7 +1199,7 @@
         <f>B25*B16/B7/C36/B4</f>
         <v>2.7961000505667102E-18</v>
       </c>
-      <c r="C40" s="5"/>
+      <c r="C40" s="4"/>
       <c r="K40" t="s">
         <v>60</v>
       </c>
@@ -1084,7 +1213,7 @@
       <c r="G41" t="s">
         <v>61</v>
       </c>
-      <c r="H41" s="6">
+      <c r="H41" s="5">
         <f>H42*H43*H45</f>
         <v>3.0822120821196141E+20</v>
       </c>
@@ -1265,4 +1394,281 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23951CBE-8CE6-4B48-8F31-8EF81147D38A}">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1E+21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="12">
+        <f>14.9-0.5*(LOG10(B2)-20)+LOG10(B3)-3</f>
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="12">
+        <f>100000</f>
+        <v>100000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="12">
+        <f>B2*B5*B5*B5*F2</f>
+        <v>6.744892276110516E-35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="12">
+        <f>B3*B5</f>
+        <v>1.6021766200000001E-14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="12">
+        <f>B13*B16/B11/B17</f>
+        <v>2.0382713634791555E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="12">
+        <v>1.6021766200000001E-19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="12">
+        <f>B18/B19</f>
+        <v>1.5541731426793828E+60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="12">
+        <v>9.1093835599999998E-31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="12">
+        <f>F5/F4</f>
+        <v>7.6249569636622952E+62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="12">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="12">
+        <f>1+(B21/B23)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="12">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="E8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8">
+        <f>EXP(F2)</f>
+        <v>13256519.14046355</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="12">
+        <v>8.8541878169999989E-12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="12">
+        <v>299792458</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="12">
+        <f>B5*B5*B5*B5</f>
+        <v>6.589334578782229E-76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="12">
+        <f>B10*B10*B10</f>
+        <v>2.6944002417373989E+25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="12">
+        <f>4*B8*B9*B9</f>
+        <v>9.8516125702040363E-22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="12">
+        <f>B6*B10*B10</f>
+        <v>8.1871056496500277E-14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="12">
+        <f>SQRT(8)</f>
+        <v>2.8284271247461903</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="12">
+        <f>B6*B6*B12</f>
+        <v>2.2358367307069281E-35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="12">
+        <f>B2*F2</f>
+        <v>1.6399999999999998E+22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="12">
+        <f>6*B8*B9*B6*B12</f>
+        <v>4.0963867321887617E-15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="12">
+        <f>B11*B20*B20</f>
+        <v>2.6357338315128916E-75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="12">
+        <f>(B7+1)/(SQRT(F6))</f>
+        <v>7.2428801232358936E-32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="12">
+        <f>1/8+(((B7+1)*(B7+1))/F6)</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="12">
+        <v>0.70710678100000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Avalanche threshold electric field calculated
</commit_message>
<xml_diff>
--- a/test/test_reference_values.xlsx
+++ b/test/test_reference_values.xlsx
@@ -1401,7 +1401,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,7 +1471,7 @@
         <v>81</v>
       </c>
       <c r="F4" s="12">
-        <f>B13*B16/B11/B17</f>
+        <f>((B13*B16)/B11)/B17</f>
         <v>2.0382713634791555E-3</v>
       </c>
     </row>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="F5" s="12">
         <f>B18/B19</f>
-        <v>1.5541731426793828E+60</v>
+        <v>1.2896663771229913</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="F6" s="12">
         <f>F5/F4</f>
-        <v>7.6249569636622952E+62</v>
+        <v>632.72555373669218</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1517,7 +1517,7 @@
       </c>
       <c r="F7" s="12">
         <f>1+(B21/B23)</f>
-        <v>1</v>
+        <v>1.1124442640510024</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1543,6 +1543,10 @@
       <c r="B9" s="12">
         <v>8.8541878169999989E-12</v>
       </c>
+      <c r="F9" s="12">
+        <f>B13*B16/B11</f>
+        <v>3.3427650361058148E+19</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1551,6 +1555,10 @@
       <c r="B10" s="12">
         <v>299792458</v>
       </c>
+      <c r="F10" s="12">
+        <f>1/B17</f>
+        <v>6.0975609756097569E-23</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1560,6 +1568,10 @@
         <f>B5*B5*B5*B5</f>
         <v>6.589334578782229E-76</v>
       </c>
+      <c r="F11" s="12">
+        <f>F9*F10</f>
+        <v>2.0382713634791555E-3</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1620,8 +1632,8 @@
         <v>84</v>
       </c>
       <c r="B18" s="12">
-        <f>6*B8*B9*B6*B12</f>
-        <v>4.0963867321887617E-15</v>
+        <f>(((6*B8)*B9)*B6*B6*B6)*B12</f>
+        <v>3.3992173015477318E-75</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1647,7 +1659,7 @@
       </c>
       <c r="B21" s="12">
         <f>(B7+1)/(SQRT(F6))</f>
-        <v>7.2428801232358936E-32</v>
+        <v>7.9510101595018284E-2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1656,7 +1668,7 @@
       </c>
       <c r="B22" s="12">
         <f>1/8+(((B7+1)*(B7+1))/F6)</f>
-        <v>0.125</v>
+        <v>0.13132185625565013</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
sixth square of a part-calculation corrected
</commit_message>
<xml_diff>
--- a/test/test_reference_values.xlsx
+++ b/test/test_reference_values.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="94">
   <si>
     <t>14.9 - 0.5 * log(electron_density * 1e-20) + log(electron_temperature * 1e-3);</t>
   </si>
@@ -302,9 +302,6 @@
   </si>
   <si>
     <t>Sixth square(1/8+(Zeff+1)^2/Trad)</t>
-  </si>
-  <si>
-    <t>Lambda</t>
   </si>
 </sst>
 </file>
@@ -1400,8 +1397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23951CBE-8CE6-4B48-8F31-8EF81147D38A}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1517,7 +1514,7 @@
       </c>
       <c r="F7" s="12">
         <f>1+(B21/B23)</f>
-        <v>1.1124442640510024</v>
+        <v>1.1115234355208197</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1528,13 +1525,6 @@
         <f>PI()</f>
         <v>3.1415926535897931</v>
       </c>
-      <c r="E8" t="s">
-        <v>94</v>
-      </c>
-      <c r="F8">
-        <f>EXP(F2)</f>
-        <v>13256519.14046355</v>
-      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1543,10 +1533,7 @@
       <c r="B9" s="12">
         <v>8.8541878169999989E-12</v>
       </c>
-      <c r="F9" s="12">
-        <f>B13*B16/B11</f>
-        <v>3.3427650361058148E+19</v>
-      </c>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1555,10 +1542,7 @@
       <c r="B10" s="12">
         <v>299792458</v>
       </c>
-      <c r="F10" s="12">
-        <f>1/B17</f>
-        <v>6.0975609756097569E-23</v>
-      </c>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1568,10 +1552,7 @@
         <f>B5*B5*B5*B5</f>
         <v>6.589334578782229E-76</v>
       </c>
-      <c r="F11" s="12">
-        <f>F9*F10</f>
-        <v>2.0382713634791555E-3</v>
-      </c>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1676,7 +1657,8 @@
         <v>93</v>
       </c>
       <c r="B23" s="12">
-        <v>0.70710678100000002</v>
+        <f>B22^(1/6)</f>
+        <v>0.71294523185823988</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Avalanche density and Runaway electron density and Avalanche generation rate calculated
</commit_message>
<xml_diff>
--- a/test/test_reference_values.xlsx
+++ b/test/test_reference_values.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="102">
   <si>
     <t>14.9 - 0.5 * log(electron_density * 1e-20) + log(electron_temperature * 1e-3);</t>
   </si>
@@ -302,6 +302,30 @@
   </si>
   <si>
     <t>Sixth square(1/8+(Zeff+1)^2/Trad)</t>
+  </si>
+  <si>
+    <t>Critical field(Ec)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electric field_2 </t>
+  </si>
+  <si>
+    <t>Electric field_1</t>
+  </si>
+  <si>
+    <t>Avalanche generation rate</t>
+  </si>
+  <si>
+    <t>Runaway electron density</t>
+  </si>
+  <si>
+    <t>A(surface)</t>
+  </si>
+  <si>
+    <t>Ir(runaway current)</t>
+  </si>
+  <si>
+    <t>Avalanche density</t>
   </si>
 </sst>
 </file>
@@ -311,7 +335,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00E+000"/>
     <numFmt numFmtId="165" formatCode="0.0000E+000"/>
-    <numFmt numFmtId="169" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.00000E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -397,7 +421,7 @@
     <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -686,7 +710,7 @@
   <dimension ref="A1:M56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A14" sqref="A14:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,9 +929,17 @@
         <f>B10*B11*B11</f>
         <v>8.1871056496500277E-14</v>
       </c>
+      <c r="C16" s="3">
+        <f>B16*B15</f>
+        <v>8.0656192931680693E-35</v>
+      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
+      <c r="C17" s="3">
+        <f>B14/C16</f>
+        <v>0.83625224932495057</v>
+      </c>
       <c r="G17" t="s">
         <v>22</v>
       </c>
@@ -921,7 +953,7 @@
         <v>23</v>
       </c>
       <c r="B18" s="3">
-        <f>B14/B15/B16</f>
+        <f>(B14/B15)/B16</f>
         <v>0.83625224932495068</v>
       </c>
     </row>
@@ -1390,15 +1422,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23951CBE-8CE6-4B48-8F31-8EF81147D38A}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1525,6 +1558,13 @@
         <f>PI()</f>
         <v>3.1415926535897931</v>
       </c>
+      <c r="E8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="12">
+        <f>B24/(B13*B14)</f>
+        <v>0.83625224932495057</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1533,7 +1573,13 @@
       <c r="B9" s="12">
         <v>8.8541878169999989E-12</v>
       </c>
-      <c r="F9" s="12"/>
+      <c r="E9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="12">
+        <f>((B26/F8)-1)/(2*F4*F2)</f>
+        <v>6.5061964275028368</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1542,7 +1588,13 @@
       <c r="B10" s="12">
         <v>299792458</v>
       </c>
-      <c r="F10" s="12"/>
+      <c r="E10" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="12">
+        <f>B27/(B28*B5*B10)</f>
+        <v>3122915017928723</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1552,7 +1604,13 @@
         <f>B5*B5*B5*B5</f>
         <v>6.589334578782229E-76</v>
       </c>
-      <c r="F11" s="12"/>
+      <c r="E11" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" s="12">
+        <f>F10/F9</f>
+        <v>479990890641975.06</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1659,6 +1717,46 @@
       <c r="B23" s="12">
         <f>B22^(1/6)</f>
         <v>0.71294523185823988</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24">
+        <v>6.744892276110516E-35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
synchrotron loss time corrected
</commit_message>
<xml_diff>
--- a/test/test_reference_values.xlsx
+++ b/test/test_reference_values.xlsx
@@ -860,10 +860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,10 +874,11 @@
     <col min="4" max="4" width="8.7109375"/>
     <col min="5" max="5" width="31.42578125"/>
     <col min="6" max="6" width="16.7109375"/>
-    <col min="7" max="1025" width="8.7109375"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>66</v>
       </c>
@@ -893,7 +894,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -908,7 +909,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -924,7 +925,7 @@
         <v>6.744892276110516E-35</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -940,7 +941,7 @@
         <v>2.038271363479156E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -955,7 +956,7 @@
         <v>1.2896663771229915</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -970,7 +971,7 @@
         <v>632.72555373669218</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -984,8 +985,12 @@
         <f>1+(B21/B23)</f>
         <v>1.1115234355208197</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="13">
+        <f>F7*F8</f>
+        <v>0.92951397313168238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -1000,8 +1005,9 @@
         <f>B24/(B13*B14)</f>
         <v>0.83625224932495079</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -1012,11 +1018,11 @@
         <v>84</v>
       </c>
       <c r="F9" s="13">
-        <f>((B26/F8)-1)/(2*F4*F2)</f>
-        <v>6.5061964275028288</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <f>((C26/F8)-1)/(2*F4*F2)</f>
+        <v>2.9915354181308507</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>85</v>
       </c>
@@ -1031,7 +1037,7 @@
         <v>3122915017928723</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -1044,10 +1050,10 @@
       </c>
       <c r="F11" s="13">
         <f>F10/F9</f>
-        <v>479990890641975.69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1043917113266190.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1063,7 +1069,7 @@
         <v>145.14409604056164</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>89</v>
       </c>
@@ -1079,7 +1085,7 @@
         <v>4.2732401843317671</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>90</v>
       </c>
@@ -1095,7 +1101,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>91</v>
       </c>
@@ -1111,7 +1117,7 @@
         <v>2.0169796938562983</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>92</v>
       </c>

</xml_diff>

<commit_message>
#36 Test reference values updated.
</commit_message>
<xml_diff>
--- a/test/test_reference_values.xlsx
+++ b/test/test_reference_values.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hadar Ádám\Documents\TortoiseSVN\runafluid\trunk\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ToDo\Munka\Runafluid\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7815" tabRatio="564" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Aval_thresh_gen_rate" sheetId="2" r:id="rId1"/>
     <sheet name="RUNAFLUID_phys_numbers" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="124">
   <si>
     <t>14.9 - 0.5 * log(electron_density * 1e-20) + log(electron_temperature * 1e-3);</t>
   </si>
@@ -377,12 +377,27 @@
   </si>
   <si>
     <t>SQRT(alpha/(alpha-1))</t>
+  </si>
+  <si>
+    <t>ref_toroidicity_dreicer_from coordinate</t>
+  </si>
+  <si>
+    <t>rho_norm</t>
+  </si>
+  <si>
+    <t>in_asp_ratio_coordinate</t>
+  </si>
+  <si>
+    <t>Dreicer Generation Rates</t>
+  </si>
+  <si>
+    <t>Ed/E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00E+000"/>
     <numFmt numFmtId="165" formatCode="0.0000E+000"/>
@@ -859,26 +874,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.140625"/>
     <col min="2" max="2" width="17.5703125"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375"/>
     <col min="5" max="5" width="31.42578125"/>
     <col min="6" max="6" width="16.7109375"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="1025" width="8.7109375"/>
+    <col min="7" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>66</v>
       </c>
@@ -894,7 +909,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -905,11 +920,11 @@
         <v>70</v>
       </c>
       <c r="F2" s="13">
-        <f>14.9-0.5*(LOG10(B2)-20)+LOG10(B3)-3</f>
-        <v>16.399999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <f>14.9-0.5*(LN(B2*POWER(10,-20)))+LN(B3*POWER(10,-3))</f>
+        <v>18.353877639491067</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -922,10 +937,10 @@
       </c>
       <c r="F3" s="13">
         <f>B2*B5*B5*B5*F2</f>
-        <v>6.744892276110516E-35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7.5484711906878547E-35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -938,10 +953,10 @@
       </c>
       <c r="F4" s="13">
         <f>((B13*B16)/B11)/B17</f>
-        <v>2.038271363479156E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.8212854535508969E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -956,7 +971,7 @@
         <v>1.2896663771229915</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -968,10 +983,10 @@
       </c>
       <c r="F6" s="13">
         <f>F5/F4</f>
-        <v>632.72555373669218</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>708.10776784527309</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -983,14 +998,14 @@
       </c>
       <c r="F7" s="13">
         <f>1+(B21/B23)</f>
-        <v>1.1115234355208197</v>
+        <v>1.1055105888710326</v>
       </c>
       <c r="G7" s="13">
         <f>F7*F8</f>
-        <v>0.92951397313168238</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.03462790986947</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -1003,11 +1018,11 @@
       </c>
       <c r="F8" s="13">
         <f>B24/(B13*B14)</f>
-        <v>0.83625224932495079</v>
+        <v>0.93588240608898254</v>
       </c>
       <c r="G8" s="13"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -1021,8 +1036,9 @@
         <f>((C26/F8)-1)/(2*F4*F2)</f>
         <v>2.9915354181308507</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>85</v>
       </c>
@@ -1037,7 +1053,7 @@
         <v>3122915017928723</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -1053,7 +1069,7 @@
         <v>1043917113266190.3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1068,8 +1084,9 @@
         <f>B29*B31*B33</f>
         <v>145.14409604056164</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>89</v>
       </c>
@@ -1082,10 +1099,10 @@
       </c>
       <c r="F13" s="13">
         <f>(F8*B14)/B4</f>
-        <v>4.2732401843317671</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4.7823492358159427</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>90</v>
       </c>
@@ -1101,7 +1118,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>91</v>
       </c>
@@ -1117,7 +1134,7 @@
         <v>2.0169796938562983</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>92</v>
       </c>
@@ -1135,7 +1152,7 @@
       </c>
       <c r="B17" s="13">
         <f>B2*F2</f>
-        <v>1.6399999999999998E+22</v>
+        <v>1.8353877639491066E+22</v>
       </c>
       <c r="E17" t="s">
         <v>114</v>
@@ -1177,7 +1194,7 @@
       </c>
       <c r="B21" s="13">
         <f>(B7+1)/(SQRT(F6))</f>
-        <v>7.9510101595018284E-2</v>
+        <v>7.5158882883148981E-2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1186,7 +1203,7 @@
       </c>
       <c r="B22" s="13">
         <f>1/8+(((B7+1)*(B7+1))/F6)</f>
-        <v>0.13132185625565013</v>
+        <v>0.1306488576762429</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1195,15 +1212,16 @@
       </c>
       <c r="B23" s="13">
         <f>B22^(1/6)</f>
-        <v>0.71294523185823988</v>
+        <v>0.71233497687153369</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
-      <c r="B24">
-        <v>6.7448922761105203E-35</v>
+      <c r="B24" s="13">
+        <f>B17*B5*B5*B5</f>
+        <v>7.5484711906878547E-35</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1223,7 +1241,7 @@
       </c>
       <c r="C26" s="13">
         <f>B26*F8</f>
-        <v>1.0035026991899409</v>
+        <v>1.1230588873067791</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1258,6 +1276,7 @@
       <c r="B30" s="15">
         <v>4.9908784068123453E-4</v>
       </c>
+      <c r="D30" s="15"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
@@ -1329,11 +1348,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S56"/>
   <sheetViews>
-    <sheetView topLeftCell="E15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView tabSelected="1" topLeftCell="C36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1355,20 +1374,26 @@
     <col min="16" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="D2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1379,8 +1404,11 @@
         <f>LOG10(B3)-20</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1391,33 +1419,40 @@
         <f>LOG10(B4)-3</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3"/>
       <c r="D6" s="3">
-        <f>14.9-0.5*(D3)+D4</f>
-        <v>16.399999999999999</v>
+        <f>14.9-0.5*(LN(B3*POWER(10,-20)))+LN(B4*POWER(10,-3))</f>
+        <v>18.353877639491067</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="5">
         <f>D6</f>
-        <v>16.399999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>18.353877639491067</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="6">
         <v>1.6021766200000001E-19</v>
+      </c>
+      <c r="D7" s="3">
+        <f>14.9-0.5*(LN(B3*POWER(10,-20)))+LN(B4*POWER(10,-3))</f>
+        <v>18.353877639491067</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>7</v>
@@ -1427,7 +1462,7 @@
         <v>4.1127391927503151E-57</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -1447,10 +1482,10 @@
       </c>
       <c r="K8">
         <f>H9*H8*(H10)^(3/2)</f>
-        <v>1.5800491986320209E-54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>1.7682944912236603E-54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -1462,14 +1497,14 @@
       </c>
       <c r="H9" s="5">
         <f>B14</f>
-        <v>6.744892276110516E-35</v>
+        <v>7.5484711906878547E-35</v>
       </c>
       <c r="I9" s="5">
         <f>H6*H7*B3</f>
-        <v>6.744892276110516E-35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>7.5484711906878547E-35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -1484,7 +1519,7 @@
         <v>9.1093835599999998E-31</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -1492,7 +1527,7 @@
         <v>299792458</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f>RUNAFLUID_phys_numbers!B1</f>
         <v>0</v>
@@ -1506,7 +1541,7 @@
       </c>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="G13" s="4" t="s">
         <v>16</v>
@@ -1523,13 +1558,13 @@
         <v>1.4117659649084197E-27</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="5">
         <f>B3*B7^3*D6</f>
-        <v>6.744892276110516E-35</v>
+        <v>7.5484711906878547E-35</v>
       </c>
       <c r="G14" t="s">
         <v>19</v>
@@ -1539,7 +1574,7 @@
         <v>2.8284271247461903</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
@@ -1548,7 +1583,7 @@
         <v>9.8516125702040401E-22</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>21</v>
       </c>
@@ -1565,14 +1600,14 @@
       <c r="B17" s="3"/>
       <c r="C17" s="3">
         <f>B14/C16</f>
-        <v>0.83625224932495024</v>
+        <v>0.93588240608898254</v>
       </c>
       <c r="G17" t="s">
         <v>22</v>
       </c>
       <c r="H17" s="3">
         <f>K8/K13</f>
-        <v>1.1192005175833216E-27</v>
+        <v>1.2525408142548389E-27</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -1581,7 +1616,7 @@
       </c>
       <c r="B18" s="3">
         <f>(B14/B15)/B16</f>
-        <v>0.83625224932495013</v>
+        <v>0.93588240608898265</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -1616,7 +1651,7 @@
       </c>
       <c r="H22" s="3">
         <f>(4*B8*B9*B9*B10*B10*H21*H21*H21)/(B3*B7*B7*B7*B7*D6)</f>
-        <v>4.9908784068123453E-4</v>
+        <v>4.4595702052414946E-4</v>
       </c>
       <c r="L22" t="s">
         <v>29</v>
@@ -1691,7 +1726,7 @@
       </c>
       <c r="H25" s="3">
         <f>Aval_thresh_gen_rate!F13</f>
-        <v>4.2732401843317671</v>
+        <v>4.7823492358159427</v>
       </c>
       <c r="L25" t="s">
         <v>36</v>
@@ -1761,7 +1796,7 @@
       </c>
       <c r="B29" s="8">
         <f>1/B3/D6</f>
-        <v>6.0975609756097557E-23</v>
+        <v>5.4484399408240193E-23</v>
       </c>
       <c r="C29" s="8"/>
     </row>
@@ -1771,7 +1806,7 @@
       </c>
       <c r="B30" s="8">
         <f>B28*B29</f>
-        <v>2.0382713634791555E-3</v>
+        <v>1.8212854535508969E-3</v>
       </c>
       <c r="C30" s="8"/>
       <c r="G30" t="s">
@@ -1783,6 +1818,12 @@
       <c r="M30">
         <f>0.5/1.65</f>
         <v>0.30303030303030304</v>
+      </c>
+      <c r="O30" t="s">
+        <v>120</v>
+      </c>
+      <c r="P30">
+        <v>0.65</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -1793,7 +1834,14 @@
       </c>
       <c r="H31">
         <f>(B3/H22)</f>
-        <v>2.0036553057174081E+24</v>
+        <v>2.2423685556618521E+24</v>
+      </c>
+      <c r="O31" t="s">
+        <v>121</v>
+      </c>
+      <c r="P31">
+        <f>M30*P30</f>
+        <v>0.19696969696969699</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -1814,7 +1862,7 @@
         <v>0.18160679263543178</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -1828,10 +1876,17 @@
       </c>
       <c r="H33" s="3">
         <f>(H25/B46)^(3*(1+B49)/16)</f>
-        <v>1.7239870089791947</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.7983138243908148</v>
+      </c>
+      <c r="L33" t="s">
+        <v>119</v>
+      </c>
+      <c r="M33">
+        <f>(1-(1.2*SQRT((2*P31)/(1+P31))))</f>
+        <v>0.31157858064052701</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -1845,77 +1900,77 @@
       </c>
       <c r="H34">
         <f>EXP(H35)</f>
-        <v>1.8467433613999357E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.3728628162402919E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
       <c r="H35" s="3">
         <f>(-1*H25/(4*B46))-(SQRT((H25*(1+B49))/B46))</f>
-        <v>-3.9917464433154066</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <v>-4.2882719795325892</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>52</v>
       </c>
       <c r="B36" s="8">
         <f>B30*B34^2</f>
-        <v>7.977595168620847E-4</v>
+        <v>7.1283334963439225E-4</v>
       </c>
       <c r="C36" s="8">
         <f>B15*B10^2*B33^3/B14/B7</f>
-        <v>4.9908784068123464E-4</v>
+        <v>4.4595702052414952E-4</v>
       </c>
       <c r="G36" t="s">
         <v>53</v>
       </c>
       <c r="H36" s="3">
         <f>H31*H32*H33*H34</f>
-        <v>2.6052449327523101E+23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.2609170748922962E+23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>54</v>
       </c>
       <c r="B39" s="8">
         <f>B25*B16/B7/B36/B4</f>
-        <v>1.749273442772706E-18</v>
+        <v>1.9576799223574102E-18</v>
       </c>
       <c r="C39" s="8">
         <f>B18*B10*B33*B33/B4</f>
-        <v>2.6796476045816915E-19</v>
+        <v>2.9988978202102277E-19</v>
       </c>
       <c r="D39" s="3">
         <f>B14/B33/B33/B10*4*B8</f>
-        <v>2.6451146221174208E-20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.9602506168763293E-20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B40" s="9">
         <f>B25*B16/B7/C36/B4</f>
-        <v>2.7961000505667086E-18</v>
+        <v>3.1292242802363517E-18</v>
       </c>
       <c r="C40" s="9"/>
       <c r="K40" t="s">
         <v>55</v>
       </c>
       <c r="L40">
-        <f>((B46*B18)/H25)</f>
-        <v>0.19569511968719822</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+        <f>((M22*B18)/H25)</f>
+        <v>0.23483414362463803</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
       <c r="G41" t="s">
@@ -1923,14 +1978,17 @@
       </c>
       <c r="H41" s="10">
         <f>H42*H43*H45</f>
-        <v>1.0517322795466147E-2</v>
+        <v>4.1377608925281709E-2</v>
+      </c>
+      <c r="K41" t="s">
+        <v>123</v>
       </c>
       <c r="L41">
         <f>1/L40</f>
-        <v>5.1099894652376303</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+        <v>4.2583245543646884</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
       <c r="G42" t="s">
@@ -1938,14 +1996,14 @@
       </c>
       <c r="H42" s="3">
         <f>1/H22</f>
-        <v>2003.6553057174081</v>
+        <v>2242.368555661852</v>
       </c>
       <c r="L42">
         <f>L41*L41</f>
-        <v>26.111992334839563</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+        <v>18.13332801030522</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
       <c r="G43" t="s">
@@ -1953,29 +2011,29 @@
       </c>
       <c r="H43" s="3">
         <f>L40^(-1*M28)</f>
-        <v>1.3314810114835549</v>
+        <v>1.2895490219262831</v>
       </c>
       <c r="L43">
         <f>L42/8</f>
-        <v>3.2639990418549454</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.2666660012881525</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
       <c r="G44" t="s">
         <v>59</v>
       </c>
       <c r="H44">
-        <f>(-1*(((M23/4)*(1/L40))+(SQRT(2*(1/L40))*M24)))</f>
-        <v>-12.443751900632357</v>
+        <f>(-1*(((M23/4)*(L41))+(SQRT(2*(L41))*M24)))</f>
+        <v>-11.154595930647321</v>
       </c>
       <c r="L44">
         <f>(2/3)*L41^1.5*SQRT(2)</f>
-        <v>10.890648618471658</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+        <v>8.2847971030547143</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
       <c r="G45" t="s">
@@ -1983,14 +2041,14 @@
       </c>
       <c r="H45">
         <f>EXP(H44)</f>
-        <v>3.9422777181689875E-6</v>
+        <v>1.4309370856773003E-5</v>
       </c>
       <c r="L45">
         <f>L44+L43</f>
-        <v>14.154647660326603</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+        <v>10.551463104342867</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>61</v>
       </c>
@@ -2000,7 +2058,7 @@
       </c>
       <c r="C46" s="8"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>62</v>
       </c>
@@ -2013,10 +2071,10 @@
       </c>
       <c r="H47" s="3">
         <f>H48*H49*H51</f>
-        <v>42.100512084959803</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+        <v>71.930862096202191</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
       <c r="G48" t="s">
@@ -2024,7 +2082,7 @@
       </c>
       <c r="H48" s="3">
         <f>H42</f>
-        <v>2003.6553057174081</v>
+        <v>2242.368555661852</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -2040,7 +2098,7 @@
       </c>
       <c r="H49" s="3">
         <f>L40^((-3/16)*(B49+1))</f>
-        <v>1.8435609559462562</v>
+        <v>1.7217279690422986</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -2051,7 +2109,7 @@
       </c>
       <c r="H50">
         <f>(-1*(((1/4)*(1/L40))+(SQRT((1+B49)*(1/L40)))))</f>
-        <v>-4.4743675436039538</v>
+        <v>-3.9829109877907749</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -2062,7 +2120,7 @@
       </c>
       <c r="H51">
         <f>EXP(H50)</f>
-        <v>1.1397428221879389E-2</v>
+        <v>1.8631324762644737E-2</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -2077,7 +2135,7 @@
       </c>
       <c r="H53" s="3">
         <f>H56*H47</f>
-        <v>21.874874399116354</v>
+        <v>9.1233364311998404</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -2092,7 +2150,7 @@
       </c>
       <c r="J54" s="3">
         <f>H54*H55</f>
-        <v>-0.65472121368008485</v>
+        <v>-2.0648698350794352</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -2100,8 +2158,8 @@
         <v>58</v>
       </c>
       <c r="H55">
-        <f>(((1/L40)*(1/L40)/8)+((2/3)*((1/L40)^(-1.5))*SQRT(1+B49)))</f>
-        <v>3.3456185045728262</v>
+        <f>(((L41)*(L41)/8)+((2/3)*((L41)^(1.5))*SQRT(1+B49)))</f>
+        <v>10.551463104342867</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -2110,7 +2168,7 @@
       </c>
       <c r="H56" s="3">
         <f>EXP(H54*H55)</f>
-        <v>0.5195868961159511</v>
+        <v>0.12683479893509486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>